<commit_message>
Actualizado template de correo de orden aprobada
</commit_message>
<xml_diff>
--- a/data/excels/eventos_prueba.xlsx
+++ b/data/excels/eventos_prueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FCO1916\Desktop\app_aapSTORE\backEndStore\data\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6416E0-D9BB-41C9-AA3B-FD50F8F7BC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5EC51A-9003-4719-B9DE-1C9B5E8E686A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6376158E-A02A-492D-B822-CAC5047F43C6}"/>
+    <workbookView minimized="1" xWindow="7545" yWindow="4530" windowWidth="21600" windowHeight="11295" xr2:uid="{6376158E-A02A-492D-B822-CAC5047F43C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -938,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E6B960-393E-4E82-A111-CAE4A6B0C75C}">
   <dimension ref="A1:AF31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>